<commit_message>
Data Provider done...Need to look at blank cells
</commit_message>
<xml_diff>
--- a/MastekBlanket/src/test/resources/testdata/Login.xlsx
+++ b/MastekBlanket/src/test/resources/testdata/Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somesh12339\Desktop\MB_New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somesh12339\Desktop\MB_New\MastekBlanket\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -42,6 +42,30 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -359,39 +383,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2">
+        <v>1111</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>